<commit_message>
update auto scs and time in ms and auto capacity
</commit_message>
<xml_diff>
--- a/Codes/dict_compose_poisson_Cl2_del_freq18.xlsx
+++ b/Codes/dict_compose_poisson_Cl2_del_freq18.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E249"/>
+  <dimension ref="A1:E179"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,16 +460,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C2" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="E2" t="n">
-        <v>0.002</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="3">
@@ -477,16 +477,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C3" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D3" t="n">
-        <v>1.71</v>
+        <v>0.36</v>
       </c>
       <c r="E3" t="n">
-        <v>0.008</v>
+        <v>0.046</v>
       </c>
     </row>
     <row r="4">
@@ -494,16 +494,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C4" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D4" t="n">
-        <v>1.11</v>
+        <v>0.41</v>
       </c>
       <c r="E4" t="n">
-        <v>0.007</v>
+        <v>0.046</v>
       </c>
     </row>
     <row r="5">
@@ -511,16 +511,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C5" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D5" t="n">
-        <v>1.5</v>
+        <v>0.34</v>
       </c>
       <c r="E5" t="n">
-        <v>0.016</v>
+        <v>0.048</v>
       </c>
     </row>
     <row r="6">
@@ -528,14 +528,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C6" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D6" t="inlineStr"/>
+        <v>1.95</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.39</v>
+      </c>
       <c r="E6" t="n">
-        <v>0.001</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="7">
@@ -543,16 +545,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C7" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D7" t="n">
-        <v>1.16</v>
+        <v>0.31</v>
       </c>
       <c r="E7" t="n">
-        <v>0.003</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="8">
@@ -560,16 +562,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C8" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D8" t="n">
-        <v>1.67</v>
+        <v>0.32</v>
       </c>
       <c r="E8" t="n">
-        <v>0.012</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="9">
@@ -577,16 +579,14 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C9" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1.61</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="n">
-        <v>0.01</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="10">
@@ -594,16 +594,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C10" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D10" t="n">
-        <v>1.22</v>
+        <v>0.38</v>
       </c>
       <c r="E10" t="n">
-        <v>0.008</v>
+        <v>0.049</v>
       </c>
     </row>
     <row r="11">
@@ -611,14 +611,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C11" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
+        <v>1.95</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.3</v>
+      </c>
       <c r="E11" t="n">
-        <v>0.001</v>
+        <v>0.018</v>
       </c>
     </row>
     <row r="12">
@@ -626,16 +628,14 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C12" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D12" t="n">
-        <v>1.73</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="n">
-        <v>0.015</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="13">
@@ -643,16 +643,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C13" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D13" t="n">
-        <v>1.53</v>
+        <v>0.42</v>
       </c>
       <c r="E13" t="n">
-        <v>0.014</v>
+        <v>0.052</v>
       </c>
     </row>
     <row r="14">
@@ -660,16 +660,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C14" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D14" t="n">
-        <v>1.49</v>
+        <v>0.4</v>
       </c>
       <c r="E14" t="n">
-        <v>0.016</v>
+        <v>0.054</v>
       </c>
     </row>
     <row r="15">
@@ -677,16 +677,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C15" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D15" t="n">
-        <v>1.15</v>
+        <v>0.33</v>
       </c>
       <c r="E15" t="n">
-        <v>0.003</v>
+        <v>0.032</v>
       </c>
     </row>
     <row r="16">
@@ -694,16 +694,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C16" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D16" t="n">
-        <v>1.82</v>
+        <v>0.27</v>
       </c>
       <c r="E16" t="n">
-        <v>0.008</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="17">
@@ -711,16 +711,14 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C17" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D17" t="n">
-        <v>1.42</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D17" t="inlineStr"/>
       <c r="E17" t="n">
-        <v>0.01</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="18">
@@ -728,10 +726,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C18" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D18" t="inlineStr"/>
       <c r="E18" t="n">
@@ -743,16 +741,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C19" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D19" t="n">
-        <v>1.56</v>
+        <v>0.49</v>
       </c>
       <c r="E19" t="n">
-        <v>0.017</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="20">
@@ -760,16 +758,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C20" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D20" t="n">
-        <v>1.78</v>
+        <v>0.45</v>
       </c>
       <c r="E20" t="n">
-        <v>0.008</v>
+        <v>0.033</v>
       </c>
     </row>
     <row r="21">
@@ -777,14 +775,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C21" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D21" t="inlineStr"/>
+        <v>1.95</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.44</v>
+      </c>
       <c r="E21" t="n">
-        <v>0.001</v>
+        <v>0.029</v>
       </c>
     </row>
     <row r="22">
@@ -792,16 +792,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C22" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D22" t="n">
-        <v>1.65</v>
+        <v>0.37</v>
       </c>
       <c r="E22" t="n">
-        <v>0.012</v>
+        <v>0.082</v>
       </c>
     </row>
     <row r="23">
@@ -809,16 +809,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C23" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D23" t="n">
-        <v>1.66</v>
+        <v>0.47</v>
       </c>
       <c r="E23" t="n">
-        <v>0.01</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="24">
@@ -826,14 +826,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C24" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D24" t="inlineStr"/>
+        <v>1.95</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.26</v>
+      </c>
       <c r="E24" t="n">
-        <v>0.001</v>
+        <v>0.013</v>
       </c>
     </row>
     <row r="25">
@@ -841,16 +843,14 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C25" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D25" t="n">
-        <v>1.09</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="26">
@@ -858,16 +858,14 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C26" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D26" t="n">
-        <v>1.33</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="n">
-        <v>0.013</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="27">
@@ -875,16 +873,14 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C27" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D27" t="n">
-        <v>1.36</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D27" t="inlineStr"/>
       <c r="E27" t="n">
-        <v>0.01</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="28">
@@ -892,16 +888,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C28" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D28" t="n">
-        <v>1.8</v>
+        <v>0.29</v>
       </c>
       <c r="E28" t="n">
-        <v>0.008</v>
+        <v>0.026</v>
       </c>
     </row>
     <row r="29">
@@ -909,16 +905,14 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C29" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D29" t="n">
-        <v>1.3</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D29" t="inlineStr"/>
       <c r="E29" t="n">
-        <v>0.013</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="30">
@@ -926,16 +920,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C30" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D30" t="n">
-        <v>1.77</v>
+        <v>0.35</v>
       </c>
       <c r="E30" t="n">
-        <v>0.011</v>
+        <v>0.059</v>
       </c>
     </row>
     <row r="31">
@@ -943,10 +937,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C31" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D31" t="inlineStr"/>
       <c r="E31" t="n">
@@ -958,16 +952,14 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C32" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D32" t="n">
-        <v>1.4</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D32" t="inlineStr"/>
       <c r="E32" t="n">
-        <v>0.015</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="33">
@@ -975,16 +967,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C33" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D33" t="n">
-        <v>1.23</v>
+        <v>0.5</v>
       </c>
       <c r="E33" t="n">
-        <v>0.012</v>
+        <v>0.007</v>
       </c>
     </row>
     <row r="34">
@@ -992,16 +984,14 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C34" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D34" t="n">
-        <v>1.44</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D34" t="inlineStr"/>
       <c r="E34" t="n">
-        <v>0.015</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="35">
@@ -1009,16 +999,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C35" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D35" t="n">
-        <v>1.29</v>
+        <v>0.48</v>
       </c>
       <c r="E35" t="n">
-        <v>0.011</v>
+        <v>0.016</v>
       </c>
     </row>
     <row r="36">
@@ -1026,16 +1016,14 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C36" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D36" t="n">
-        <v>1.35</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D36" t="inlineStr"/>
       <c r="E36" t="n">
-        <v>0.016</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="37">
@@ -1043,16 +1031,14 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C37" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D37" t="n">
-        <v>1.14</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="n">
-        <v>0.013</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="38">
@@ -1060,16 +1046,14 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C38" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D38" t="n">
-        <v>1.95</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="39">
@@ -1077,16 +1061,14 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C39" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D39" t="n">
-        <v>1.51</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D39" t="inlineStr"/>
       <c r="E39" t="n">
-        <v>0.014</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="40">
@@ -1094,10 +1076,10 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C40" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D40" t="inlineStr"/>
       <c r="E40" t="n">
@@ -1109,16 +1091,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C41" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D41" t="n">
-        <v>1.62</v>
+        <v>0.43</v>
       </c>
       <c r="E41" t="n">
-        <v>0.017</v>
+        <v>0.036</v>
       </c>
     </row>
     <row r="42">
@@ -1126,16 +1108,14 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C42" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D42" t="n">
-        <v>1.59</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="n">
-        <v>0.01</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="43">
@@ -1143,16 +1123,14 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C43" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D43" t="n">
-        <v>1.64</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D43" t="inlineStr"/>
       <c r="E43" t="n">
-        <v>0.011</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="44">
@@ -1160,14 +1138,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C44" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D44" t="inlineStr"/>
+        <v>1.95</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.46</v>
+      </c>
       <c r="E44" t="n">
-        <v>0.001</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="45">
@@ -1175,16 +1155,14 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C45" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D45" t="n">
-        <v>1.48</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D45" t="inlineStr"/>
       <c r="E45" t="n">
-        <v>0.019</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="46">
@@ -1192,16 +1170,14 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C46" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D46" t="n">
-        <v>1.01</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D46" t="inlineStr"/>
       <c r="E46" t="n">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="47">
@@ -1209,16 +1185,14 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C47" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D47" t="n">
-        <v>1.55</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D47" t="inlineStr"/>
       <c r="E47" t="n">
-        <v>0.013</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="48">
@@ -1226,16 +1200,14 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C48" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D48" t="n">
-        <v>1.38</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D48" t="inlineStr"/>
       <c r="E48" t="n">
-        <v>0.012</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="49">
@@ -1243,16 +1215,14 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C49" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D49" t="n">
-        <v>1.58</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D49" t="inlineStr"/>
       <c r="E49" t="n">
-        <v>0.02</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="50">
@@ -1260,10 +1230,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C50" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D50" t="inlineStr"/>
       <c r="E50" t="n">
@@ -1275,16 +1245,14 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C51" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D51" t="n">
-        <v>1.74</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D51" t="inlineStr"/>
       <c r="E51" t="n">
-        <v>0.008</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="52">
@@ -1292,16 +1260,14 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C52" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D52" t="n">
-        <v>1.26</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D52" t="inlineStr"/>
       <c r="E52" t="n">
-        <v>0.01</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="53">
@@ -1309,16 +1275,14 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C53" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D53" t="n">
-        <v>1.86</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D53" t="inlineStr"/>
       <c r="E53" t="n">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="54">
@@ -1326,16 +1290,14 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C54" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D54" t="n">
-        <v>1.2</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D54" t="inlineStr"/>
       <c r="E54" t="n">
-        <v>0.008</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="55">
@@ -1343,16 +1305,14 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C55" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D55" t="n">
-        <v>1.41</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D55" t="inlineStr"/>
       <c r="E55" t="n">
-        <v>0.013</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="56">
@@ -1360,16 +1320,14 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C56" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D56" t="n">
-        <v>1.39</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D56" t="inlineStr"/>
       <c r="E56" t="n">
-        <v>0.01</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="57">
@@ -1377,14 +1335,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C57" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D57" t="inlineStr"/>
+        <v>1.95</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.28</v>
+      </c>
       <c r="E57" t="n">
-        <v>0.001</v>
+        <v>0.008999999999999999</v>
       </c>
     </row>
     <row r="58">
@@ -1392,10 +1352,10 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C58" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="n">
@@ -1407,16 +1367,14 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C59" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D59" t="n">
-        <v>1.6</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D59" t="inlineStr"/>
       <c r="E59" t="n">
-        <v>0.021</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="60">
@@ -1424,16 +1382,14 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C60" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D60" t="n">
-        <v>1.81</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D60" t="inlineStr"/>
       <c r="E60" t="n">
-        <v>0.008</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="61">
@@ -1441,10 +1397,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C61" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D61" t="inlineStr"/>
       <c r="E61" t="n">
@@ -1456,16 +1412,14 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C62" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D62" t="n">
-        <v>1.02</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D62" t="inlineStr"/>
       <c r="E62" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="63">
@@ -1473,16 +1427,14 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C63" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D63" t="n">
-        <v>1.69</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D63" t="inlineStr"/>
       <c r="E63" t="n">
-        <v>0.012</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="64">
@@ -1490,16 +1442,14 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C64" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D64" t="n">
-        <v>1.54</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D64" t="inlineStr"/>
       <c r="E64" t="n">
-        <v>0.012</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="65">
@@ -1507,16 +1457,14 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C65" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D65" t="n">
-        <v>1.32</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D65" t="inlineStr"/>
       <c r="E65" t="n">
-        <v>0.006</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="66">
@@ -1524,10 +1472,10 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C66" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="n">
@@ -1539,16 +1487,14 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C67" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D67" t="n">
-        <v>1.25</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D67" t="inlineStr"/>
       <c r="E67" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="68">
@@ -1556,16 +1502,14 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C68" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D68" t="n">
-        <v>1.34</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D68" t="inlineStr"/>
       <c r="E68" t="n">
-        <v>0.015</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="69">
@@ -1573,10 +1517,10 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C69" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="n">
@@ -1588,16 +1532,14 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C70" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D70" t="n">
-        <v>1.97</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D70" t="inlineStr"/>
       <c r="E70" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="71">
@@ -1605,16 +1547,14 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C71" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D71" t="n">
-        <v>1.79</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D71" t="inlineStr"/>
       <c r="E71" t="n">
-        <v>0.006</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="72">
@@ -1622,16 +1562,14 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C72" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D72" t="n">
-        <v>1.21</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D72" t="inlineStr"/>
       <c r="E72" t="n">
-        <v>0.007</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="73">
@@ -1639,16 +1577,14 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C73" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D73" t="n">
-        <v>1.57</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D73" t="inlineStr"/>
       <c r="E73" t="n">
-        <v>0.021</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="74">
@@ -1656,16 +1592,14 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C74" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D74" t="n">
-        <v>1.9</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D74" t="inlineStr"/>
       <c r="E74" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="75">
@@ -1673,10 +1607,10 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C75" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="n">
@@ -1688,16 +1622,14 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C76" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D76" t="n">
-        <v>1.87</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D76" t="inlineStr"/>
       <c r="E76" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="77">
@@ -1705,16 +1637,14 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C77" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D77" t="n">
-        <v>1.98</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D77" t="inlineStr"/>
       <c r="E77" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="78">
@@ -1722,16 +1652,14 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C78" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D78" t="n">
-        <v>1.43</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D78" t="inlineStr"/>
       <c r="E78" t="n">
-        <v>0.015</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="79">
@@ -1739,10 +1667,10 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C79" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="n">
@@ -1754,16 +1682,14 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C80" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D80" t="n">
-        <v>1.91</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D80" t="inlineStr"/>
       <c r="E80" t="n">
-        <v>0.007</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="81">
@@ -1771,16 +1697,14 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C81" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D81" t="n">
-        <v>1.92</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D81" t="inlineStr"/>
       <c r="E81" t="n">
-        <v>0.006</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="82">
@@ -1788,16 +1712,14 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C82" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D82" t="n">
-        <v>1.94</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D82" t="inlineStr"/>
       <c r="E82" t="n">
-        <v>0.004</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="83">
@@ -1805,10 +1727,10 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C83" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="n">
@@ -1820,10 +1742,10 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C84" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="n">
@@ -1835,10 +1757,10 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C85" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="n">
@@ -1850,10 +1772,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C86" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="n">
@@ -1865,16 +1787,14 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C87" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D87" t="n">
-        <v>1.76</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D87" t="inlineStr"/>
       <c r="E87" t="n">
-        <v>0.012</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="88">
@@ -1882,10 +1802,10 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C88" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="n">
@@ -1897,16 +1817,14 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C89" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D89" t="n">
-        <v>1.47</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D89" t="inlineStr"/>
       <c r="E89" t="n">
-        <v>0.018</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="90">
@@ -1914,16 +1832,14 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C90" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D90" t="n">
-        <v>1.12</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D90" t="inlineStr"/>
       <c r="E90" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="91">
@@ -1931,16 +1847,14 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C91" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D91" t="n">
-        <v>1.46</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D91" t="inlineStr"/>
       <c r="E91" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="92">
@@ -1948,16 +1862,14 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C92" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D92" t="n">
-        <v>1.45</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D92" t="inlineStr"/>
       <c r="E92" t="n">
-        <v>0.013</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="93">
@@ -1965,16 +1877,14 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C93" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D93" t="n">
-        <v>1.1</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D93" t="inlineStr"/>
       <c r="E93" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="94">
@@ -1982,10 +1892,10 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C94" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="n">
@@ -1997,16 +1907,14 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C95" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D95" t="n">
-        <v>1.37</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D95" t="inlineStr"/>
       <c r="E95" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="96">
@@ -2014,10 +1922,10 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C96" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="n">
@@ -2029,16 +1937,14 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C97" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D97" t="n">
-        <v>1.17</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D97" t="inlineStr"/>
       <c r="E97" t="n">
-        <v>0.011</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="98">
@@ -2046,10 +1952,10 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C98" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="n">
@@ -2061,16 +1967,14 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C99" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D99" t="n">
-        <v>1.68</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D99" t="inlineStr"/>
       <c r="E99" t="n">
-        <v>0.01</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="100">
@@ -2078,16 +1982,14 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C100" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D100" t="n">
-        <v>1.83</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D100" t="inlineStr"/>
       <c r="E100" t="n">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="101">
@@ -2095,10 +1997,10 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C101" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="n">
@@ -2110,10 +2012,10 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C102" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="n">
@@ -2125,16 +2027,14 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C103" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D103" t="n">
-        <v>1.96</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D103" t="inlineStr"/>
       <c r="E103" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="104">
@@ -2142,16 +2042,14 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C104" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D104" t="n">
-        <v>1.27</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D104" t="inlineStr"/>
       <c r="E104" t="n">
-        <v>0.007</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="105">
@@ -2159,16 +2057,14 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C105" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D105" t="n">
-        <v>1.63</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D105" t="inlineStr"/>
       <c r="E105" t="n">
-        <v>0.008</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="106">
@@ -2176,16 +2072,14 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C106" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D106" t="n">
-        <v>1.75</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D106" t="inlineStr"/>
       <c r="E106" t="n">
-        <v>0.006</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="107">
@@ -2193,10 +2087,10 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C107" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D107" t="inlineStr"/>
       <c r="E107" t="n">
@@ -2208,10 +2102,10 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C108" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D108" t="inlineStr"/>
       <c r="E108" t="n">
@@ -2223,16 +2117,14 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C109" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D109" t="n">
-        <v>1.52</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D109" t="inlineStr"/>
       <c r="E109" t="n">
-        <v>0.008</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="110">
@@ -2240,16 +2132,14 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C110" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D110" t="n">
-        <v>1.03</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D110" t="inlineStr"/>
       <c r="E110" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="111">
@@ -2257,14 +2147,12 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C111" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D111" t="n">
-        <v>1.07</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D111" t="inlineStr"/>
       <c r="E111" t="n">
         <v>0.001</v>
       </c>
@@ -2274,10 +2162,10 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C112" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D112" t="inlineStr"/>
       <c r="E112" t="n">
@@ -2289,10 +2177,10 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C113" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D113" t="inlineStr"/>
       <c r="E113" t="n">
@@ -2304,10 +2192,10 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C114" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D114" t="inlineStr"/>
       <c r="E114" t="n">
@@ -2319,16 +2207,14 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C115" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D115" t="n">
-        <v>1.72</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D115" t="inlineStr"/>
       <c r="E115" t="n">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="116">
@@ -2336,10 +2222,10 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C116" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D116" t="inlineStr"/>
       <c r="E116" t="n">
@@ -2351,10 +2237,10 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C117" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D117" t="inlineStr"/>
       <c r="E117" t="n">
@@ -2366,10 +2252,10 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C118" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D118" t="inlineStr"/>
       <c r="E118" t="n">
@@ -2381,16 +2267,14 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C119" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D119" t="n">
-        <v>1.28</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D119" t="inlineStr"/>
       <c r="E119" t="n">
-        <v>0.007</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="120">
@@ -2398,10 +2282,10 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C120" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D120" t="inlineStr"/>
       <c r="E120" t="n">
@@ -2413,10 +2297,10 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C121" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D121" t="inlineStr"/>
       <c r="E121" t="n">
@@ -2428,10 +2312,10 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C122" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D122" t="inlineStr"/>
       <c r="E122" t="n">
@@ -2443,10 +2327,10 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C123" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D123" t="inlineStr"/>
       <c r="E123" t="n">
@@ -2458,10 +2342,10 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C124" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D124" t="inlineStr"/>
       <c r="E124" t="n">
@@ -2473,10 +2357,10 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C125" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D125" t="inlineStr"/>
       <c r="E125" t="n">
@@ -2488,10 +2372,10 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C126" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D126" t="inlineStr"/>
       <c r="E126" t="n">
@@ -2503,10 +2387,10 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C127" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D127" t="inlineStr"/>
       <c r="E127" t="n">
@@ -2518,16 +2402,14 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C128" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D128" t="n">
-        <v>1.04</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D128" t="inlineStr"/>
       <c r="E128" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="129">
@@ -2535,10 +2417,10 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C129" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D129" t="inlineStr"/>
       <c r="E129" t="n">
@@ -2550,10 +2432,10 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C130" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D130" t="inlineStr"/>
       <c r="E130" t="n">
@@ -2565,10 +2447,10 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C131" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D131" t="inlineStr"/>
       <c r="E131" t="n">
@@ -2580,10 +2462,10 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C132" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D132" t="inlineStr"/>
       <c r="E132" t="n">
@@ -2595,10 +2477,10 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C133" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D133" t="inlineStr"/>
       <c r="E133" t="n">
@@ -2610,10 +2492,10 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C134" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D134" t="inlineStr"/>
       <c r="E134" t="n">
@@ -2625,10 +2507,10 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C135" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D135" t="inlineStr"/>
       <c r="E135" t="n">
@@ -2640,10 +2522,10 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C136" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D136" t="inlineStr"/>
       <c r="E136" t="n">
@@ -2655,10 +2537,10 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C137" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D137" t="inlineStr"/>
       <c r="E137" t="n">
@@ -2670,10 +2552,10 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C138" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D138" t="inlineStr"/>
       <c r="E138" t="n">
@@ -2685,10 +2567,10 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C139" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D139" t="inlineStr"/>
       <c r="E139" t="n">
@@ -2700,10 +2582,10 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C140" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D140" t="inlineStr"/>
       <c r="E140" t="n">
@@ -2715,14 +2597,12 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C141" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D141" t="n">
-        <v>1.93</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D141" t="inlineStr"/>
       <c r="E141" t="n">
         <v>0.001</v>
       </c>
@@ -2732,16 +2612,14 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C142" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D142" t="n">
-        <v>1.18</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D142" t="inlineStr"/>
       <c r="E142" t="n">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="143">
@@ -2749,10 +2627,10 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C143" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D143" t="inlineStr"/>
       <c r="E143" t="n">
@@ -2764,10 +2642,10 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C144" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D144" t="inlineStr"/>
       <c r="E144" t="n">
@@ -2779,10 +2657,10 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C145" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D145" t="inlineStr"/>
       <c r="E145" t="n">
@@ -2794,10 +2672,10 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C146" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D146" t="inlineStr"/>
       <c r="E146" t="n">
@@ -2809,10 +2687,10 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C147" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D147" t="inlineStr"/>
       <c r="E147" t="n">
@@ -2824,10 +2702,10 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C148" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D148" t="inlineStr"/>
       <c r="E148" t="n">
@@ -2839,10 +2717,10 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C149" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D149" t="inlineStr"/>
       <c r="E149" t="n">
@@ -2854,10 +2732,10 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C150" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D150" t="inlineStr"/>
       <c r="E150" t="n">
@@ -2869,10 +2747,10 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C151" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D151" t="inlineStr"/>
       <c r="E151" t="n">
@@ -2884,10 +2762,10 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C152" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D152" t="inlineStr"/>
       <c r="E152" t="n">
@@ -2899,10 +2777,10 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C153" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D153" t="inlineStr"/>
       <c r="E153" t="n">
@@ -2914,10 +2792,10 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C154" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D154" t="inlineStr"/>
       <c r="E154" t="n">
@@ -2929,10 +2807,10 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C155" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D155" t="inlineStr"/>
       <c r="E155" t="n">
@@ -2944,10 +2822,10 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C156" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D156" t="inlineStr"/>
       <c r="E156" t="n">
@@ -2959,16 +2837,14 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C157" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D157" t="n">
-        <v>1.7</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D157" t="inlineStr"/>
       <c r="E157" t="n">
-        <v>0.006</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="158">
@@ -2976,16 +2852,14 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C158" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D158" t="n">
-        <v>1.05</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D158" t="inlineStr"/>
       <c r="E158" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="159">
@@ -2993,16 +2867,14 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C159" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D159" t="n">
-        <v>1.24</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D159" t="inlineStr"/>
       <c r="E159" t="n">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="160">
@@ -3010,10 +2882,10 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C160" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D160" t="inlineStr"/>
       <c r="E160" t="n">
@@ -3025,10 +2897,10 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C161" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D161" t="inlineStr"/>
       <c r="E161" t="n">
@@ -3040,16 +2912,14 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C162" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D162" t="n">
-        <v>1.88</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D162" t="inlineStr"/>
       <c r="E162" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="163">
@@ -3057,16 +2927,14 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C163" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D163" t="n">
-        <v>1.06</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D163" t="inlineStr"/>
       <c r="E163" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="164">
@@ -3074,10 +2942,10 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C164" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D164" t="inlineStr"/>
       <c r="E164" t="n">
@@ -3089,16 +2957,14 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C165" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D165" t="n">
-        <v>1.19</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D165" t="inlineStr"/>
       <c r="E165" t="n">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="166">
@@ -3106,10 +2972,10 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C166" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D166" t="inlineStr"/>
       <c r="E166" t="n">
@@ -3121,10 +2987,10 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C167" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D167" t="inlineStr"/>
       <c r="E167" t="n">
@@ -3136,10 +3002,10 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C168" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D168" t="inlineStr"/>
       <c r="E168" t="n">
@@ -3151,14 +3017,12 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C169" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D169" t="n">
-        <v>1.85</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D169" t="inlineStr"/>
       <c r="E169" t="n">
         <v>0.001</v>
       </c>
@@ -3168,10 +3032,10 @@
         <v>168</v>
       </c>
       <c r="B170" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C170" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D170" t="inlineStr"/>
       <c r="E170" t="n">
@@ -3183,10 +3047,10 @@
         <v>169</v>
       </c>
       <c r="B171" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C171" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D171" t="inlineStr"/>
       <c r="E171" t="n">
@@ -3198,16 +3062,14 @@
         <v>170</v>
       </c>
       <c r="B172" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C172" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D172" t="n">
-        <v>1.31</v>
-      </c>
+        <v>1.95</v>
+      </c>
+      <c r="D172" t="inlineStr"/>
       <c r="E172" t="n">
-        <v>0.005</v>
+        <v>0.001</v>
       </c>
     </row>
     <row r="173">
@@ -3215,10 +3077,10 @@
         <v>171</v>
       </c>
       <c r="B173" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C173" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D173" t="inlineStr"/>
       <c r="E173" t="n">
@@ -3230,10 +3092,10 @@
         <v>172</v>
       </c>
       <c r="B174" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C174" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D174" t="inlineStr"/>
       <c r="E174" t="n">
@@ -3245,10 +3107,10 @@
         <v>173</v>
       </c>
       <c r="B175" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C175" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D175" t="inlineStr"/>
       <c r="E175" t="n">
@@ -3260,10 +3122,10 @@
         <v>174</v>
       </c>
       <c r="B176" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C176" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D176" t="inlineStr"/>
       <c r="E176" t="n">
@@ -3275,10 +3137,10 @@
         <v>175</v>
       </c>
       <c r="B177" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C177" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D177" t="inlineStr"/>
       <c r="E177" t="n">
@@ -3290,10 +3152,10 @@
         <v>176</v>
       </c>
       <c r="B178" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C178" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D178" t="inlineStr"/>
       <c r="E178" t="n">
@@ -3305,1073 +3167,13 @@
         <v>177</v>
       </c>
       <c r="B179" t="n">
-        <v>8.159722222222223</v>
+        <v>33.94444444444444</v>
       </c>
       <c r="C179" t="n">
-        <v>1.875</v>
+        <v>1.95</v>
       </c>
       <c r="D179" t="inlineStr"/>
       <c r="E179" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="180">
-      <c r="A180" s="1" t="n">
-        <v>178</v>
-      </c>
-      <c r="B180" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C180" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D180" t="inlineStr"/>
-      <c r="E180" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="181">
-      <c r="A181" s="1" t="n">
-        <v>179</v>
-      </c>
-      <c r="B181" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C181" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D181" t="inlineStr"/>
-      <c r="E181" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="B182" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C182" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D182" t="inlineStr"/>
-      <c r="E182" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="1" t="n">
-        <v>181</v>
-      </c>
-      <c r="B183" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C183" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D183" t="inlineStr"/>
-      <c r="E183" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" s="1" t="n">
-        <v>182</v>
-      </c>
-      <c r="B184" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C184" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D184" t="inlineStr"/>
-      <c r="E184" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" s="1" t="n">
-        <v>183</v>
-      </c>
-      <c r="B185" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C185" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D185" t="inlineStr"/>
-      <c r="E185" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" s="1" t="n">
-        <v>184</v>
-      </c>
-      <c r="B186" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C186" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D186" t="inlineStr"/>
-      <c r="E186" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="187">
-      <c r="A187" s="1" t="n">
-        <v>185</v>
-      </c>
-      <c r="B187" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C187" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D187" t="n">
-        <v>1.08</v>
-      </c>
-      <c r="E187" t="n">
-        <v>0.002</v>
-      </c>
-    </row>
-    <row r="188">
-      <c r="A188" s="1" t="n">
-        <v>186</v>
-      </c>
-      <c r="B188" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C188" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D188" t="inlineStr"/>
-      <c r="E188" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="189">
-      <c r="A189" s="1" t="n">
-        <v>187</v>
-      </c>
-      <c r="B189" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C189" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D189" t="inlineStr"/>
-      <c r="E189" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="190">
-      <c r="A190" s="1" t="n">
-        <v>188</v>
-      </c>
-      <c r="B190" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C190" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D190" t="inlineStr"/>
-      <c r="E190" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="191">
-      <c r="A191" s="1" t="n">
-        <v>189</v>
-      </c>
-      <c r="B191" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C191" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D191" t="inlineStr"/>
-      <c r="E191" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="192">
-      <c r="A192" s="1" t="n">
-        <v>190</v>
-      </c>
-      <c r="B192" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C192" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D192" t="inlineStr"/>
-      <c r="E192" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="193">
-      <c r="A193" s="1" t="n">
-        <v>191</v>
-      </c>
-      <c r="B193" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C193" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D193" t="inlineStr"/>
-      <c r="E193" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="194">
-      <c r="A194" s="1" t="n">
-        <v>192</v>
-      </c>
-      <c r="B194" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C194" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D194" t="n">
-        <v>1.84</v>
-      </c>
-      <c r="E194" t="n">
-        <v>0.004</v>
-      </c>
-    </row>
-    <row r="195">
-      <c r="A195" s="1" t="n">
-        <v>193</v>
-      </c>
-      <c r="B195" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C195" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D195" t="inlineStr"/>
-      <c r="E195" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="196">
-      <c r="A196" s="1" t="n">
-        <v>194</v>
-      </c>
-      <c r="B196" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C196" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D196" t="inlineStr"/>
-      <c r="E196" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="197">
-      <c r="A197" s="1" t="n">
-        <v>195</v>
-      </c>
-      <c r="B197" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C197" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D197" t="n">
-        <v>1.13</v>
-      </c>
-      <c r="E197" t="n">
-        <v>0.008999999999999999</v>
-      </c>
-    </row>
-    <row r="198">
-      <c r="A198" s="1" t="n">
-        <v>196</v>
-      </c>
-      <c r="B198" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C198" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D198" t="inlineStr"/>
-      <c r="E198" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="199">
-      <c r="A199" s="1" t="n">
-        <v>197</v>
-      </c>
-      <c r="B199" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C199" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D199" t="inlineStr"/>
-      <c r="E199" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="200">
-      <c r="A200" s="1" t="n">
-        <v>198</v>
-      </c>
-      <c r="B200" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C200" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D200" t="inlineStr"/>
-      <c r="E200" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="201">
-      <c r="A201" s="1" t="n">
-        <v>199</v>
-      </c>
-      <c r="B201" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C201" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D201" t="inlineStr"/>
-      <c r="E201" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" s="1" t="n">
-        <v>200</v>
-      </c>
-      <c r="B202" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C202" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D202" t="inlineStr"/>
-      <c r="E202" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" s="1" t="n">
-        <v>201</v>
-      </c>
-      <c r="B203" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C203" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D203" t="inlineStr"/>
-      <c r="E203" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" s="1" t="n">
-        <v>202</v>
-      </c>
-      <c r="B204" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C204" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D204" t="inlineStr"/>
-      <c r="E204" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" s="1" t="n">
-        <v>203</v>
-      </c>
-      <c r="B205" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C205" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D205" t="inlineStr"/>
-      <c r="E205" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" s="1" t="n">
-        <v>204</v>
-      </c>
-      <c r="B206" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C206" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D206" t="inlineStr"/>
-      <c r="E206" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" s="1" t="n">
-        <v>205</v>
-      </c>
-      <c r="B207" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C207" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D207" t="inlineStr"/>
-      <c r="E207" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" s="1" t="n">
-        <v>206</v>
-      </c>
-      <c r="B208" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C208" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D208" t="inlineStr"/>
-      <c r="E208" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" s="1" t="n">
-        <v>207</v>
-      </c>
-      <c r="B209" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C209" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D209" t="inlineStr"/>
-      <c r="E209" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" s="1" t="n">
-        <v>208</v>
-      </c>
-      <c r="B210" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C210" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D210" t="inlineStr"/>
-      <c r="E210" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" s="1" t="n">
-        <v>209</v>
-      </c>
-      <c r="B211" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C211" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D211" t="inlineStr"/>
-      <c r="E211" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" s="1" t="n">
-        <v>210</v>
-      </c>
-      <c r="B212" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C212" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D212" t="inlineStr"/>
-      <c r="E212" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" s="1" t="n">
-        <v>211</v>
-      </c>
-      <c r="B213" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C213" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D213" t="inlineStr"/>
-      <c r="E213" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" s="1" t="n">
-        <v>212</v>
-      </c>
-      <c r="B214" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C214" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D214" t="inlineStr"/>
-      <c r="E214" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" s="1" t="n">
-        <v>213</v>
-      </c>
-      <c r="B215" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C215" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D215" t="inlineStr"/>
-      <c r="E215" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" s="1" t="n">
-        <v>214</v>
-      </c>
-      <c r="B216" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C216" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D216" t="n">
-        <v>1.99</v>
-      </c>
-      <c r="E216" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" s="1" t="n">
-        <v>215</v>
-      </c>
-      <c r="B217" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C217" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D217" t="inlineStr"/>
-      <c r="E217" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" s="1" t="n">
-        <v>216</v>
-      </c>
-      <c r="B218" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C218" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D218" t="inlineStr"/>
-      <c r="E218" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" s="1" t="n">
-        <v>217</v>
-      </c>
-      <c r="B219" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C219" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D219" t="inlineStr"/>
-      <c r="E219" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" s="1" t="n">
-        <v>218</v>
-      </c>
-      <c r="B220" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C220" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D220" t="inlineStr"/>
-      <c r="E220" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" s="1" t="n">
-        <v>219</v>
-      </c>
-      <c r="B221" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C221" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D221" t="inlineStr"/>
-      <c r="E221" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" s="1" t="n">
-        <v>220</v>
-      </c>
-      <c r="B222" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C222" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D222" t="inlineStr"/>
-      <c r="E222" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" s="1" t="n">
-        <v>221</v>
-      </c>
-      <c r="B223" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C223" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D223" t="inlineStr"/>
-      <c r="E223" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" s="1" t="n">
-        <v>222</v>
-      </c>
-      <c r="B224" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C224" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D224" t="inlineStr"/>
-      <c r="E224" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" s="1" t="n">
-        <v>223</v>
-      </c>
-      <c r="B225" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C225" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D225" t="inlineStr"/>
-      <c r="E225" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" s="1" t="n">
-        <v>224</v>
-      </c>
-      <c r="B226" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C226" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D226" t="inlineStr"/>
-      <c r="E226" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" s="1" t="n">
-        <v>225</v>
-      </c>
-      <c r="B227" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C227" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D227" t="inlineStr"/>
-      <c r="E227" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" s="1" t="n">
-        <v>226</v>
-      </c>
-      <c r="B228" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C228" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D228" t="inlineStr"/>
-      <c r="E228" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" s="1" t="n">
-        <v>227</v>
-      </c>
-      <c r="B229" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C229" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D229" t="inlineStr"/>
-      <c r="E229" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" s="1" t="n">
-        <v>228</v>
-      </c>
-      <c r="B230" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C230" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D230" t="inlineStr"/>
-      <c r="E230" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" s="1" t="n">
-        <v>229</v>
-      </c>
-      <c r="B231" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C231" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D231" t="inlineStr"/>
-      <c r="E231" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" s="1" t="n">
-        <v>230</v>
-      </c>
-      <c r="B232" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C232" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D232" t="inlineStr"/>
-      <c r="E232" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" s="1" t="n">
-        <v>231</v>
-      </c>
-      <c r="B233" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C233" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D233" t="inlineStr"/>
-      <c r="E233" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" s="1" t="n">
-        <v>232</v>
-      </c>
-      <c r="B234" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C234" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D234" t="inlineStr"/>
-      <c r="E234" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" s="1" t="n">
-        <v>233</v>
-      </c>
-      <c r="B235" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C235" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D235" t="inlineStr"/>
-      <c r="E235" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" s="1" t="n">
-        <v>234</v>
-      </c>
-      <c r="B236" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C236" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D236" t="inlineStr"/>
-      <c r="E236" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" s="1" t="n">
-        <v>235</v>
-      </c>
-      <c r="B237" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C237" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D237" t="inlineStr"/>
-      <c r="E237" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" s="1" t="n">
-        <v>236</v>
-      </c>
-      <c r="B238" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C238" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D238" t="inlineStr"/>
-      <c r="E238" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" s="1" t="n">
-        <v>237</v>
-      </c>
-      <c r="B239" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C239" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D239" t="inlineStr"/>
-      <c r="E239" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" s="1" t="n">
-        <v>238</v>
-      </c>
-      <c r="B240" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C240" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D240" t="inlineStr"/>
-      <c r="E240" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" s="1" t="n">
-        <v>239</v>
-      </c>
-      <c r="B241" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C241" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D241" t="inlineStr"/>
-      <c r="E241" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" s="1" t="n">
-        <v>240</v>
-      </c>
-      <c r="B242" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C242" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D242" t="inlineStr"/>
-      <c r="E242" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" s="1" t="n">
-        <v>241</v>
-      </c>
-      <c r="B243" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C243" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D243" t="n">
-        <v>2</v>
-      </c>
-      <c r="E243" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" s="1" t="n">
-        <v>242</v>
-      </c>
-      <c r="B244" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C244" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D244" t="inlineStr"/>
-      <c r="E244" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" s="1" t="n">
-        <v>243</v>
-      </c>
-      <c r="B245" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C245" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D245" t="inlineStr"/>
-      <c r="E245" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" s="1" t="n">
-        <v>244</v>
-      </c>
-      <c r="B246" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C246" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D246" t="inlineStr"/>
-      <c r="E246" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" s="1" t="n">
-        <v>245</v>
-      </c>
-      <c r="B247" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C247" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D247" t="inlineStr"/>
-      <c r="E247" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" s="1" t="n">
-        <v>246</v>
-      </c>
-      <c r="B248" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C248" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D248" t="inlineStr"/>
-      <c r="E248" t="n">
-        <v>0.001</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" s="1" t="n">
-        <v>247</v>
-      </c>
-      <c r="B249" t="n">
-        <v>8.159722222222223</v>
-      </c>
-      <c r="C249" t="n">
-        <v>1.875</v>
-      </c>
-      <c r="D249" t="inlineStr"/>
-      <c r="E249" t="n">
         <v>0.001</v>
       </c>
     </row>

</xml_diff>